<commit_message>
Update 10. Funções Mercado de Trabalho
Anotações e Prática. Aulas da 60 à 61.
</commit_message>
<xml_diff>
--- a/10. Funções Mercado de Trabalho/Funções Mercado de Trabalho - Função CORRESP.xlsx
+++ b/10. Funções Mercado de Trabalho/Funções Mercado de Trabalho - Função CORRESP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kiko\Documents\Projetos Programação\Especializacao-em-Analise-de-Dados\10. Funções Mercado de Trabalho\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF371EA1-36D0-4ED0-B492-5696971D6C51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B914573C-3F6E-4E02-9B25-B57F2FF3E094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{90D394A7-0334-4363-9DA1-420D95C76B52}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{90D394A7-0334-4363-9DA1-420D95C76B52}"/>
   </bookViews>
   <sheets>
     <sheet name="CORRESP" sheetId="2" r:id="rId1"/>
@@ -3874,7 +3874,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14320F23-E21A-4F4C-B9C0-5DAADE102FA6}">
   <dimension ref="A1:G309"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -5270,7 +5270,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58476F61-E96E-445D-B26A-359D96FCABAF}">
   <dimension ref="A1:I309"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -5363,7 +5365,7 @@
         <v>Produto 5</v>
       </c>
       <c r="I4" s="1" t="str">
-        <f>INDEX(A:A,MATCH($G$1,B:B,0))</f>
+        <f>INDEX(A2:A16,MATCH(G1,B2:B16,0))</f>
         <v>Produto 5</v>
       </c>
     </row>
@@ -5387,12 +5389,12 @@
         <f t="shared" ref="G5:G6" si="0">MATCH($G$1,$B$2:$B$16,0)</f>
         <v>5</v>
       </c>
-      <c r="H5" s="5" cm="1">
+      <c r="H5" s="4" cm="1">
         <f t="array" ref="H5">INDEX($C$2:$C$16,G5)</f>
         <v>6228</v>
       </c>
-      <c r="I5" s="5">
-        <f>INDEX(C:C,MATCH($G$1,B:B,0))</f>
+      <c r="I5" s="4">
+        <f>INDEX(C2:C16,MATCH(G1,B2:B16,0))</f>
         <v>6228</v>
       </c>
     </row>
@@ -5421,7 +5423,7 @@
         <v>Alpha</v>
       </c>
       <c r="I6" s="1" t="str">
-        <f>INDEX(D:D,MATCH($G$1,B:B,0))</f>
+        <f>INDEX(D2:D16,MATCH(G1,B2:B16,0))</f>
         <v>Alpha</v>
       </c>
     </row>
@@ -6689,7 +6691,7 @@
       <c r="C309" s="2"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1" xr:uid="{7D0A6B31-66D5-48D4-A8CA-2C12940921FF}">
       <formula1>$B$2:$B$16</formula1>
     </dataValidation>

</xml_diff>